<commit_message>
created functions for show values, show null counts
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac2d22d054a0a418/DSI/Projects/Predicting-Loan-Defaults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16463\OneDrive\DSI\Projects\Predicting-Loan-Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{BE6FA9DB-FF90-4F3F-B9BC-C2B37A92C9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24425762-1B22-433A-8D04-489491802B0B}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{BE6FA9DB-FF90-4F3F-B9BC-C2B37A92C9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F403ECEC-FBB4-4DCF-85FE-4A2FE857863E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4580" yWindow="6160" windowWidth="7500" windowHeight="6750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$B$1:$C$152</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$C$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="140001"/>
@@ -2267,14 +2267,14 @@
   <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="32.6328125" customWidth="1"/>
-    <col min="3" max="3" width="196.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.6328125" customWidth="1"/>
     <col min="4" max="4" width="118.81640625" style="6" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
   </cols>
@@ -2922,7 +2922,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B71" s="9" t="s">
         <v>121</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B118" s="18" t="s">
         <v>312</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B119" s="18" t="s">
         <v>314</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B120" s="18" t="s">
         <v>316</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B121" s="18" t="s">
         <v>318</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B122" s="18" t="s">
         <v>320</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B123" s="18" t="s">
         <v>322</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B124" s="18" t="s">
         <v>324</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B125" s="18" t="s">
         <v>336</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B126" s="18" t="s">
         <v>327</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B127" s="18" t="s">
         <v>329</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B128" s="18" t="s">
         <v>331</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B129" s="18" t="s">
         <v>333</v>
       </c>
@@ -3586,21 +3586,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C152" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:C152" xr:uid="{607435C3-4CB4-4FD4-8B07-68370CDFFCB9}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="sec_app_chargeoff_within_12_mths"/>
-        <filter val="sec_app_collections_12_mths_ex_med"/>
-        <filter val="sec_app_earliest_cr_line"/>
-        <filter val="sec_app_fico_range_high"/>
-        <filter val="sec_app_fico_range_low"/>
-        <filter val="sec_app_inq_last_6mths"/>
-        <filter val="sec_app_mort_acc"/>
-        <filter val="sec_app_mths_since_last_major_derog"/>
-        <filter val="sec_app_num_rev_accts"/>
-        <filter val="sec_app_open_acc"/>
-        <filter val="sec_app_open_act_il"/>
-        <filter val="sec_app_revol_util"/>
+        <filter val="num_tl_120dpd_2m"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3608,7 +3597,7 @@
     <sortCondition ref="B2:B101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
data cleaning on target variable, removing features, created conditional columns, currently working on imputing null values code.
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16463\OneDrive\DSI\Projects\Predicting-Loan-Defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{BE6FA9DB-FF90-4F3F-B9BC-C2B37A92C9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F403ECEC-FBB4-4DCF-85FE-4A2FE857863E}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{BE6FA9DB-FF90-4F3F-B9BC-C2B37A92C9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B874B7CA-AACE-4D81-9444-30E63FF4A30D}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4580" yWindow="6160" windowWidth="7500" windowHeight="6750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -22,10 +22,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$C$152</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2268,7 +2274,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2353,7 +2359,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>114</v>
       </c>
@@ -2922,7 +2928,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71" s="9" t="s">
         <v>121</v>
       </c>
@@ -3589,7 +3595,7 @@
   <autoFilter ref="A1:C152" xr:uid="{607435C3-4CB4-4FD4-8B07-68370CDFFCB9}">
     <filterColumn colId="1">
       <filters>
-        <filter val="num_tl_120dpd_2m"/>
+        <filter val="avg_cur_bal"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>